<commit_message>
Approval and Part mapping
</commit_message>
<xml_diff>
--- a/assets/formats/Parts.xlsx
+++ b/assets/formats/Parts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PRTMS_NEW\assets\formats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,78 +35,15 @@
     <t>Electrical</t>
   </si>
   <si>
-    <t>ELP001</t>
-  </si>
-  <si>
-    <t>ELP002</t>
-  </si>
-  <si>
-    <t>ELP003</t>
-  </si>
-  <si>
-    <t>ELP004</t>
-  </si>
-  <si>
-    <t>EL Part 1</t>
-  </si>
-  <si>
-    <t>EL Part 2</t>
-  </si>
-  <si>
-    <t>EL Part 3</t>
-  </si>
-  <si>
-    <t>EL Part 4</t>
-  </si>
-  <si>
     <t>Mechanical</t>
   </si>
   <si>
-    <t>MCP005</t>
-  </si>
-  <si>
-    <t>MCP006</t>
-  </si>
-  <si>
-    <t>MCP007</t>
-  </si>
-  <si>
-    <t>MC Part 1</t>
-  </si>
-  <si>
-    <t>MC Part 2</t>
-  </si>
-  <si>
-    <t>MC Part 3</t>
-  </si>
-  <si>
     <t>Part Category</t>
   </si>
   <si>
     <t>Part Number</t>
   </si>
   <si>
-    <t>Part no1</t>
-  </si>
-  <si>
-    <t>Part no2</t>
-  </si>
-  <si>
-    <t>Part no3</t>
-  </si>
-  <si>
-    <t>Part no4</t>
-  </si>
-  <si>
-    <t>Part no5</t>
-  </si>
-  <si>
-    <t>Part no6</t>
-  </si>
-  <si>
-    <t>Part no7</t>
-  </si>
-  <si>
     <t>img_file</t>
   </si>
   <si>
@@ -129,6 +66,69 @@
   </si>
   <si>
     <t>img7.jpg</t>
+  </si>
+  <si>
+    <t>num1</t>
+  </si>
+  <si>
+    <t>num2</t>
+  </si>
+  <si>
+    <t>num3</t>
+  </si>
+  <si>
+    <t>num4</t>
+  </si>
+  <si>
+    <t>num5</t>
+  </si>
+  <si>
+    <t>num6</t>
+  </si>
+  <si>
+    <t>ELP00111</t>
+  </si>
+  <si>
+    <t>ELP00112</t>
+  </si>
+  <si>
+    <t>ELP00113</t>
+  </si>
+  <si>
+    <t>ELP00114</t>
+  </si>
+  <si>
+    <t>ELP00115</t>
+  </si>
+  <si>
+    <t>ELP00116</t>
+  </si>
+  <si>
+    <t>ELP00117</t>
+  </si>
+  <si>
+    <t>EL Part 111</t>
+  </si>
+  <si>
+    <t>EL Part 112</t>
+  </si>
+  <si>
+    <t>EL Part 113</t>
+  </si>
+  <si>
+    <t>EL Part 114</t>
+  </si>
+  <si>
+    <t>EL Part 115</t>
+  </si>
+  <si>
+    <t>EL Part 116</t>
+  </si>
+  <si>
+    <t>EL Part 117</t>
+  </si>
+  <si>
+    <t>num76</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +516,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -525,10 +525,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -536,108 +536,108 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>